<commit_message>
removed one comment that was unnecessery
</commit_message>
<xml_diff>
--- a/cladevo/static/uploads/(9)193_219_261_383_429_508_626_18_642.xlsx
+++ b/cladevo/static/uploads/(9)193_219_261_383_429_508_626_18_642.xlsx
@@ -534,7 +534,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +545,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF5983B0"/>
       </patternFill>
     </fill>
     <fill>
@@ -561,8 +573,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -607,7 +625,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,35 +646,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,7 +729,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -717,7 +759,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -846,7 +888,7 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -896,13 +938,13 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -914,19 +956,19 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -941,16 +983,16 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="3" t="s">
@@ -967,7 +1009,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="1" t="n">
@@ -1047,7 +1089,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -1127,7 +1169,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -1207,7 +1249,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -1287,7 +1329,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1" t="n">
@@ -1367,247 +1409,247 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="1" t="n">
+      <c r="B7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="1" t="n">
+      <c r="B8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="1" t="n">
+      <c r="B9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1" t="n">
@@ -1687,7 +1729,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -1767,7 +1809,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="1" t="n">
@@ -1847,87 +1889,87 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="1" t="n">
+      <c r="B13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="1" t="n">
@@ -2007,7 +2049,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="1" t="n">
@@ -2087,7 +2129,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="1" t="n">
@@ -2167,7 +2209,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="1" t="n">
@@ -2247,7 +2289,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="1" t="n">
@@ -2327,7 +2369,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="1" t="n">
@@ -2407,7 +2449,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="1" t="n">
@@ -2487,7 +2529,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="1" t="n">
@@ -2567,7 +2609,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="1" t="n">
@@ -2647,7 +2689,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="1" t="n">
@@ -2727,7 +2769,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="1" t="n">
@@ -2807,7 +2849,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="1" t="n">
@@ -2887,7 +2929,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="1" t="n">
@@ -2967,7 +3009,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -3047,7 +3089,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="1" t="n">
@@ -3127,7 +3169,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -3207,7 +3249,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="1" t="n">
@@ -3287,7 +3329,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="18" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -3367,7 +3409,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="1" t="n">
@@ -3447,7 +3489,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="1" t="n">

</xml_diff>